<commit_message>
updated up to 17-jun
</commit_message>
<xml_diff>
--- a/03. Mar/29-Mar-25.xlsx
+++ b/03. Mar/29-Mar-25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\03. Mar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FD58BF-5AE5-4BA5-89EA-D34A5C8F3C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B18EBE-F841-4D90-9178-C63BF6B1AF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,9 +166,6 @@
     <t>67.77%</t>
   </si>
   <si>
-    <t>JKL-U2</t>
-  </si>
-  <si>
     <t>65.3%</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>JKL2</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +664,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">TODAY() - 11</f>
-        <v>45745</v>
+        <v>45799</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="75" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6">
         <v>57655</v>
@@ -1238,10 +1238,10 @@
         <v>10.220000000000001</v>
       </c>
       <c r="R10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="T10" s="6">
         <v>27610504</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7">
         <v>280988</v>
@@ -1312,10 +1312,10 @@
         <v>10.52</v>
       </c>
       <c r="R11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="T11" s="7">
         <v>102686541</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6">
         <v>74181</v>
@@ -1386,10 +1386,10 @@
         <v>10.17</v>
       </c>
       <c r="R12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S12" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="T12" s="6">
         <v>14734280</v>
@@ -1409,27 +1409,27 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1454,10 +1454,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="9">
         <v>315000</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="9">
         <v>350000</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="9">
         <v>385000</v>
@@ -1514,10 +1514,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="9">
         <v>420000</v>
@@ -1534,10 +1534,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="9">
         <v>455000</v>
@@ -1567,22 +1567,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,10 +1607,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6">
         <v>315000</v>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6">
         <v>350000</v>
@@ -1647,10 +1647,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6">
         <v>385000</v>
@@ -1667,10 +1667,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6">
         <v>420000</v>
@@ -1687,10 +1687,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6">
         <v>455000</v>

</xml_diff>